<commit_message>
v0.6.0 Actualizacion e Insercion de datos
</commit_message>
<xml_diff>
--- a/modulo/resultados_query.xlsx
+++ b/modulo/resultados_query.xlsx
@@ -623,7 +623,7 @@
         </is>
       </c>
       <c r="I3" t="n">
-        <v>502</v>
+        <v>123</v>
       </c>
       <c r="J3" t="n">
         <v>1</v>
@@ -675,7 +675,7 @@
         </is>
       </c>
       <c r="I4" t="n">
-        <v>502</v>
+        <v>908</v>
       </c>
       <c r="J4" t="n">
         <v>1</v>
@@ -727,7 +727,7 @@
         </is>
       </c>
       <c r="I5" t="n">
-        <v>502</v>
+        <v>111</v>
       </c>
       <c r="J5" t="n">
         <v>1</v>
@@ -765,7 +765,7 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>9000571@hotmail.com</t>
+          <t xml:space="preserve">9000571@hotmail.com </t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
@@ -779,7 +779,7 @@
         </is>
       </c>
       <c r="I6" t="n">
-        <v>502</v>
+        <v>754</v>
       </c>
       <c r="J6" t="n">
         <v>1</v>

</xml_diff>